<commit_message>
More Updates to hardware
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Dev/445L/lab-7-and-10-project-nnat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Dev\ECE445L\lab-7-and-10-project-nnat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77639552-F65C-A74F-A45D-0F2E481DB44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA92931-B2CD-49C0-971A-1E834A417C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>Quantity</t>
   </si>
@@ -330,6 +330,60 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>M61P103KT20</t>
+  </si>
+  <si>
+    <t>72-M61P103KT20</t>
+  </si>
+  <si>
+    <t>Potentiometers 61 P 10K 10% TU50 e3</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>AC/DC WALL MNT ADAPTER 5.9V 12W</t>
+  </si>
+  <si>
+    <t>Triad Magnetics</t>
+  </si>
+  <si>
+    <t>WSU060-2000</t>
+  </si>
+  <si>
+    <t>Digkey</t>
+  </si>
+  <si>
+    <t>237-2014-ND</t>
+  </si>
+  <si>
+    <t>U5, U6</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U8, U9, U10, U11, U12, U13, U14</t>
   </si>
 </sst>
 </file>
@@ -468,7 +522,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -498,13 +552,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="8" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -917,27 +964,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB64E12-2F57-4D15-BA8D-127B966BFCD4}">
-  <dimension ref="A1:Q84"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="135" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="65.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="11.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="65.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.36328125" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="1"/>
+    <col min="8" max="8" width="24.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -955,7 +1002,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -971,7 +1018,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -983,7 +1030,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -994,7 +1041,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1032,734 +1079,645 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="2">
         <v>11.55</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="2">
         <f>A6*I6</f>
         <v>11.55</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="J7" s="2">
+        <f>A7*I7</f>
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="3">
+        <v>12935</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I9" s="2">
         <v>0.19</v>
       </c>
-      <c r="J7" s="14">
-        <f>A7*I7</f>
+      <c r="J9" s="2">
+        <f>A9*I9</f>
         <v>0.19</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13" t="s">
+      <c r="B10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I10" s="2">
         <v>11.06</v>
       </c>
-      <c r="J8" s="14">
-        <f>A8*I8</f>
+      <c r="J10" s="2">
+        <f>A10*I10</f>
         <v>22.12</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J11" s="2">
+        <f>A11*I11</f>
+        <v>0.9</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
+      <c r="B12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I12" s="12">
         <v>3.9089999999999998</v>
       </c>
-      <c r="J9" s="14">
-        <f t="shared" ref="J9:J10" si="0">A9*I9</f>
+      <c r="J12" s="2">
+        <f>A12*I12</f>
         <v>27.363</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
         <v>1</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="14">
-        <v>0.9</v>
-      </c>
-      <c r="J10" s="14">
-        <f t="shared" si="0"/>
-        <v>0.9</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="3">
+        <v>358</v>
+      </c>
+      <c r="I13" s="2">
+        <v>19.96</v>
+      </c>
+      <c r="J13" s="2">
+        <f>A13*I13</f>
+        <v>19.96</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="13">
-        <v>358</v>
-      </c>
-      <c r="I11" s="14">
-        <v>19.96</v>
-      </c>
-      <c r="J11" s="14">
-        <f>A11*I11</f>
-        <v>19.96</v>
-      </c>
-      <c r="K11" s="12" t="s">
+      <c r="C14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
         <v>16</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
+      <c r="C15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="J15" s="2">
+        <f>I15*A15</f>
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="14">
-        <v>1.68</v>
-      </c>
-      <c r="J12" s="14">
-        <f>A12*I12</f>
-        <v>1.68</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
-        <v>1</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="13">
-        <v>12935</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="14">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
-        <v>16</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="15">
-        <v>0.18</v>
-      </c>
-      <c r="J14" s="14">
-        <f>I14*A14</f>
-        <v>2.88</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="5:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
-      <c r="P49" s="12"/>
-      <c r="Q49" s="12"/>
-    </row>
-    <row r="50" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="12"/>
-      <c r="Q50" s="12"/>
-    </row>
-    <row r="51" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
-    </row>
-    <row r="52" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-      <c r="O52" s="12"/>
-      <c r="P52" s="12"/>
-      <c r="Q52" s="12"/>
-    </row>
-    <row r="53" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-    </row>
-    <row r="54" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
-    </row>
-    <row r="55" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-    </row>
-    <row r="56" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="H56" s="1"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-    </row>
-    <row r="57" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-    </row>
-    <row r="58" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-    </row>
-    <row r="59" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="12"/>
-      <c r="P59" s="12"/>
-      <c r="Q59" s="12"/>
-    </row>
-    <row r="60" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
-      <c r="P60" s="12"/>
-      <c r="Q60" s="12"/>
-    </row>
-    <row r="61" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-    </row>
-    <row r="62" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-    </row>
-    <row r="63" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="12"/>
-      <c r="Q63" s="12"/>
-    </row>
-    <row r="64" spans="5:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:8" x14ac:dyDescent="0.35">
       <c r="F80" s="1"/>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="H84" s="11"/>
@@ -1789,128 +1747,128 @@
       <selection activeCell="E18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>

</xml_diff>

<commit_message>
Lab7A Schematic and BOM - Ashton
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Dev\ECE445L\lab-7-and-10-project-nnat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA92931-B2CD-49C0-971A-1E834A417C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11144611-5E22-49FB-A9F7-02A54F963FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
+    <workbookView xWindow="-38520" yWindow="3360" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="BOM" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$5:$J$5</definedName>
@@ -95,8 +96,126 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ECE_IT</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{61DBC324-3237-4758-883A-A8DABF8F9B3A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ECE_IT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+How many are on your board. If 0, it should probably not clutter your bom up…
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{A5F2425F-FAB4-4F61-857F-FD82068F629A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ECE_IT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is something like C1, R2 , U1, etc. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ECE_IT</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{2DC2083D-E7E5-49AF-9E90-E093D21FACBC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ECE_IT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+How many are on your board. If 0, it should probably not clutter your bom up…
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{BB68435B-D105-4A7F-AC7F-1F845944B963}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ECE_IT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is something like C1, R2 , U1, etc. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="291">
   <si>
     <t>Quantity</t>
   </si>
@@ -311,9 +430,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>BB</t>
-  </si>
-  <si>
     <t>Good-Ark Semiconductor</t>
   </si>
   <si>
@@ -384,6 +500,678 @@
   </si>
   <si>
     <t>U8, U9, U10, U11, U12, U13, U14</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>1.0u</t>
+  </si>
+  <si>
+    <t>0.01u</t>
+  </si>
+  <si>
+    <t>2.2u</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>10p</t>
+  </si>
+  <si>
+    <t>C9, C10</t>
+  </si>
+  <si>
+    <t>C5, C11</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>C12, C13</t>
+  </si>
+  <si>
+    <t>27n</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Power Raiting</t>
+  </si>
+  <si>
+    <t>1.2n</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>Type/Dielectric</t>
+  </si>
+  <si>
+    <t>C15, C16, C27, C28</t>
+  </si>
+  <si>
+    <t>C6, C7, C17, C29</t>
+  </si>
+  <si>
+    <t>C18, C30</t>
+  </si>
+  <si>
+    <t>C19, C20, C31, C32</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4,  C14, C22, C23, C24, C25, C26, C33, C34, C35, C36, C37, C38</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>200k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES </t>
+  </si>
+  <si>
+    <t>75k</t>
+  </si>
+  <si>
+    <t>R5, R11, R17, R33, R39, R45</t>
+  </si>
+  <si>
+    <t>R21, R22, R49, R50</t>
+  </si>
+  <si>
+    <t>R6, R7, R15, R16, R23, R24, R25,R26, R27, R28, R34, R35, R43, R44, R51, R52, R53, R54, R55, R56</t>
+  </si>
+  <si>
+    <t>R58, R59</t>
+  </si>
+  <si>
+    <t>R60</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R61</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R8, R9, R10, R12, R13, R14, R18, R19, R20, R29, R30, R31, R32, R36, R37, R38, R40, R41, R42, R46, R47, R48, R62, R63, R65,  R66, R67, R68, R69</t>
+  </si>
+  <si>
+    <t>POT</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 500MA TO220-3</t>
+  </si>
+  <si>
+    <t>TO220-3</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>500mA</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>LM2937ET-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>926-LM2937ET-3.3NOPB</t>
+  </si>
+  <si>
+    <t>D1, D2</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>1.2V</t>
+  </si>
+  <si>
+    <t>DIODE STANDARD 75V 200MA DO204AH</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>200mA</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>1N914</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Onsemi</t>
+  </si>
+  <si>
+    <t>512-1N914</t>
+  </si>
+  <si>
+    <t>Checkout Window</t>
+  </si>
+  <si>
+    <t>R76, R77</t>
+  </si>
+  <si>
+    <t>D3, D4</t>
+  </si>
+  <si>
+    <t>20mA</t>
+  </si>
+  <si>
+    <t>1.6V</t>
+  </si>
+  <si>
+    <t>LED RED DIFFUSED T-1 3/4 T/H</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Broadcom Limited</t>
+  </si>
+  <si>
+    <t>516-1323-ND</t>
+  </si>
+  <si>
+    <t>HLMP-D150</t>
+  </si>
+  <si>
+    <t>R70, R71, R72, R73, R74, R75, R76, R80</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>50R</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>CONN</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>P120PK-Y25BR10K</t>
+  </si>
+  <si>
+    <t>TT Electrtonics/BI</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>X7R</t>
+  </si>
+  <si>
+    <t>50V</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL10B104KB8NFNC</t>
+  </si>
+  <si>
+    <t>187-CL10B104KB8NFNC</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 10V X7R 0603</t>
+  </si>
+  <si>
+    <t>MSAST168SB7105KTNA01</t>
+  </si>
+  <si>
+    <t>963-MSAST168SB7105KT</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>25V</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Tant</t>
+  </si>
+  <si>
+    <t>CAP CER 10PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>C0G/NP0</t>
+  </si>
+  <si>
+    <t>Walsin Technology Corporation</t>
+  </si>
+  <si>
+    <t>0603N100F500CT</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM1885C1H103JA01J</t>
+  </si>
+  <si>
+    <t>81-GRM1885C1H103JA1J</t>
+  </si>
+  <si>
+    <t>16V</t>
+  </si>
+  <si>
+    <t>GRM21BR71C475KE51L</t>
+  </si>
+  <si>
+    <t>81-GRM21BR71C475KE1L</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>791-0603N100F500CT</t>
+  </si>
+  <si>
+    <t>791-0603B273K250CT</t>
+  </si>
+  <si>
+    <t>CAP CER 0.027UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>0603B273K250CT</t>
+  </si>
+  <si>
+    <t>3.6n</t>
+  </si>
+  <si>
+    <t>81-GRM1885C1H362JA1D</t>
+  </si>
+  <si>
+    <t>CAP CER 3600PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>GRM1885C1H362JA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 1200PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>GRM1885C1H122JA01D</t>
+  </si>
+  <si>
+    <t>81-GRM1885C1H122JA01</t>
+  </si>
+  <si>
+    <t>187-CL21B106KPQNNNE</t>
+  </si>
+  <si>
+    <t>CL21B106KPQNNNE</t>
+  </si>
+  <si>
+    <t>10V</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X7R 0805</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0</t>
+  </si>
+  <si>
+    <t>708-RNCP0603FTD10K0</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>Thin Film</t>
+  </si>
+  <si>
+    <t>1/8W</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>708-RNCP0603FTD20K0</t>
+  </si>
+  <si>
+    <t>RES 20K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD20K0</t>
+  </si>
+  <si>
+    <t>708-RNCF0603DTE100K</t>
+  </si>
+  <si>
+    <t>RNCF0603DTE100K</t>
+  </si>
+  <si>
+    <t>Thin FIlm</t>
+  </si>
+  <si>
+    <t>1/6W</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 0.5% 1/6W 0603</t>
+  </si>
+  <si>
+    <t>Thick Film</t>
+  </si>
+  <si>
+    <t>603-RC0603DR-07200KL</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>RC0603DR-07200KL</t>
+  </si>
+  <si>
+    <t>1/10W</t>
+  </si>
+  <si>
+    <t>RES 200K OHM 0.5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>603-AF0603FR-0775KL</t>
+  </si>
+  <si>
+    <t>AF0603FR-0775KL</t>
+  </si>
+  <si>
+    <t>RES SMD 75K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>660-RK73B2ATTDD510J</t>
+  </si>
+  <si>
+    <t>RES SMD 51 OHM 5% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>1/4W</t>
+  </si>
+  <si>
+    <t>Thick FIlm</t>
+  </si>
+  <si>
+    <t>KOA Speer</t>
+  </si>
+  <si>
+    <t>RK73B2ATTDD510J</t>
+  </si>
+  <si>
+    <t>660-RN73R1JTD1001D25</t>
+  </si>
+  <si>
+    <t>KOA Speer Electronics, Inc.</t>
+  </si>
+  <si>
+    <t>RN73R1JTTD1001D25</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 0.5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>603-AC0603FR-1047KL</t>
+  </si>
+  <si>
+    <t>RES 47K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>AC0603FR-1047KL</t>
+  </si>
+  <si>
+    <t>603-RC0603JR-071MP</t>
+  </si>
+  <si>
+    <t>RC0603JR-071MP</t>
+  </si>
+  <si>
+    <t>RES 1M OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>858-P120PKY25BR10K</t>
+  </si>
+  <si>
+    <t>POT 10K OHM 1/20W PLASTIC LINEAR</t>
+  </si>
+  <si>
+    <t>1/20W</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>708-RNCP0603FTD2K00</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD2K00</t>
+  </si>
+  <si>
+    <t>2 kOhms ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Anti-Sulfur Thin Film</t>
+  </si>
+  <si>
+    <t>Already Owned</t>
+  </si>
+  <si>
+    <t>McDurmot</t>
+  </si>
+  <si>
+    <t>8DIP</t>
+  </si>
+  <si>
+    <t>TO92-3</t>
+  </si>
+  <si>
+    <t>8-DIP</t>
+  </si>
+  <si>
+    <t>ABM3-16.000MHZ-B2-T</t>
+  </si>
+  <si>
+    <t>535-9103-1-ND</t>
+  </si>
+  <si>
+    <t>48QFN</t>
+  </si>
+  <si>
+    <t>CONN JACK STEREO 3.5MM TH R/A</t>
+  </si>
+  <si>
+    <t>Kycon, Inc.</t>
+  </si>
+  <si>
+    <t>STX-3000</t>
+  </si>
+  <si>
+    <t>806-STX-3000</t>
+  </si>
+  <si>
+    <t>C21, C40</t>
+  </si>
+  <si>
+    <t>R57, R81</t>
+  </si>
+  <si>
+    <t>ST7735R</t>
+  </si>
+  <si>
+    <t>Adafruit Industries LLC</t>
+  </si>
+  <si>
+    <t>DISPL GRAPHIC 1.8 CLR TFT SHIELD</t>
+  </si>
+  <si>
+    <t>1528-1352-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 36000POS 2.54MM</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>77311-418-00LF</t>
+  </si>
+  <si>
+    <t>609-77311-418-00LFCT-ND</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>CRY</t>
+  </si>
+  <si>
+    <t>16.000MHZ</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16.0000MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>5POS</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 2.1X5.5MM SOLDER</t>
+  </si>
+  <si>
+    <t>Würth Elektronik</t>
+  </si>
+  <si>
+    <t>694106301002</t>
+  </si>
+  <si>
+    <t>710-694106301002</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Professor" means ask your professor quantity and style will vary </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(bring a print out of your SCH circuit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"Box means in box in your professor's office (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bring a print out of your SCH circuit</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>U5, U15</t>
+  </si>
+  <si>
+    <t>KYOCERA AVX</t>
+  </si>
+  <si>
+    <t>F931E225KAA</t>
+  </si>
+  <si>
+    <t>647-F931E225KAA</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>CAP TANT 2.2UF 10% 25V 1206</t>
   </si>
 </sst>
 </file>
@@ -395,7 +1183,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -491,6 +1279,63 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF6600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -522,7 +1367,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -555,6 +1400,39 @@
     </xf>
     <xf numFmtId="8" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -966,25 +1844,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB64E12-2F57-4D15-BA8D-127B966BFCD4}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P23" sqref="A1:P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="65.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="11.453125" style="1"/>
+    <col min="8" max="8" width="24.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -1002,7 +1880,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -1018,7 +1896,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1030,7 +1908,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1041,7 +1919,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1079,12 +1957,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -1115,12 +1993,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -1148,12 +2026,12 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -1162,7 +2040,7 @@
         <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="3">
         <v>12935</v>
@@ -1180,12 +2058,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
@@ -1216,12 +2094,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
@@ -1252,12 +2130,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
@@ -1288,12 +2166,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -1324,7 +2202,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -1357,35 +2235,32 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I15" s="12">
         <v>0.18</v>
@@ -1395,329 +2270,329 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I16" s="2">
         <v>2.81</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F80" s="1"/>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="H84" s="11"/>
@@ -1740,144 +2615,2675 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F259CE0-00F5-4859-8537-F4B5EB7CD0DC}">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F259CE0-00F5-4859-8537-F4B5EB7CD0DC}">
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="A1:E18"/>
+      <selection activeCell="A6" sqref="A6:K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="70.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6">
+        <v>45664</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="E4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="2">
+        <v>11.55</v>
+      </c>
+      <c r="J6" s="2">
+        <f>A6*I6</f>
+        <v>11.55</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.68</v>
+      </c>
+      <c r="J7" s="2">
+        <f>A7*I7</f>
+        <v>1.68</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="3">
+        <v>12935</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="2">
+        <v>11.06</v>
+      </c>
+      <c r="J10" s="2">
+        <f>A10*I10</f>
+        <v>22.12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J11" s="2">
+        <f>A11*I11</f>
+        <v>0.9</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="12">
+        <v>3.9089999999999998</v>
+      </c>
+      <c r="J12" s="2">
+        <f>A12*I12</f>
+        <v>27.363</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="3">
+        <v>358</v>
+      </c>
+      <c r="I13" s="2">
+        <v>19.96</v>
+      </c>
+      <c r="J13" s="2">
+        <f>A13*I13</f>
+        <v>19.96</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="J15" s="2">
+        <f>I15*A15</f>
+        <v>2.88</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2.81</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" location="common_component_prefixes" display="Reference Designator" xr:uid="{15F363C0-DE92-4DF8-B9BB-C0511AB47104}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029DCE93-6AF6-4E19-8B76-EC8302CAC997}">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20">
+        <v>45664</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="19"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>16</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="N6" s="18">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O6" s="18">
+        <f>N6*A6</f>
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="N7" s="18">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="O7" s="18">
+        <f t="shared" ref="O7:O9" si="0">N7*A7</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="N8" s="18">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="O8" s="18">
+        <f t="shared" si="0"/>
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>1</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="G9" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="N9" s="18">
+        <v>2.08</v>
+      </c>
+      <c r="O9" s="18">
+        <f t="shared" si="0"/>
+        <v>2.08</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>2</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O10" s="18">
+        <f>A10*N10</f>
+        <v>0.05</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>2</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="N11" s="18">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="O11" s="18">
+        <f>A11*N11</f>
+        <v>0.104</v>
+      </c>
+      <c r="P11" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>4</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="N12" s="18">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O12" s="18">
+        <f t="shared" ref="O12:O26" si="1">A12*N12</f>
+        <v>0.1</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>2</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="O13" s="18">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="P13" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>4</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="N14" s="18">
+        <v>2.7E-2</v>
+      </c>
+      <c r="O14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.108</v>
+      </c>
+      <c r="P14" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="N15" s="18">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O15" s="18">
+        <f t="shared" si="1"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="P15" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>33</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="N16" s="18">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O16" s="18">
+        <f t="shared" si="1"/>
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="P16" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>6</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="N17" s="18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="O17" s="18">
+        <f t="shared" si="1"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="P17" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>20</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="29">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="N18" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="O18" s="18">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="P18" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>4</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="29">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19" s="18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O19" s="18">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>2</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="N20" s="18">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O20" s="18">
+        <f t="shared" si="1"/>
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="P20" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
+        <v>2</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="N21" s="18">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O21" s="18">
+        <f t="shared" si="1"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="P21" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
+        <v>1</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="29">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="N22" s="18">
+        <v>5.5E-2</v>
+      </c>
+      <c r="O22" s="18">
+        <f t="shared" si="1"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="P22" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
+        <v>1</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="N23" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="O23" s="18">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="P23" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
+        <v>1</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="N24" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="O24" s="18">
+        <f t="shared" si="1"/>
+        <v>0.01</v>
+      </c>
+      <c r="P24" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>8</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="N25" s="18">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="O25" s="18">
+        <f t="shared" si="1"/>
+        <v>8.1359999999999992</v>
+      </c>
+      <c r="P25" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="N26" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="O26" s="18">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="P26" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="16">
+        <v>1</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27" s="17">
+        <v>11.55</v>
+      </c>
+      <c r="O27" s="17">
+        <v>0</v>
+      </c>
+      <c r="P27" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
+        <v>1</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M28" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="N28" s="17">
+        <v>1.68</v>
+      </c>
+      <c r="O28" s="17">
+        <v>0</v>
+      </c>
+      <c r="P28" s="18" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
+        <v>1</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K29" s="16">
+        <v>12935</v>
+      </c>
+      <c r="L29" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="O29" s="17">
+        <v>0</v>
+      </c>
+      <c r="P29" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="16">
+        <v>1</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="N30" s="17">
+        <v>1.45</v>
+      </c>
+      <c r="O30" s="17">
+        <v>0</v>
+      </c>
+      <c r="P30" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
+        <v>2</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N31" s="17">
+        <v>11.06</v>
+      </c>
+      <c r="O31" s="17">
+        <v>0</v>
+      </c>
+      <c r="P31" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="16">
+        <v>1</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N32" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="O32" s="17">
+        <v>0</v>
+      </c>
+      <c r="P32" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="16">
+        <v>7</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="N33" s="12">
+        <v>3.9089999999999998</v>
+      </c>
+      <c r="O33" s="17">
+        <v>0</v>
+      </c>
+      <c r="P33" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="16">
+        <v>1</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="L34" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="N34" s="17">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="O34" s="17">
+        <v>0</v>
+      </c>
+      <c r="P34" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="16">
+        <v>2</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="K35" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M35" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="N35" s="17">
+        <v>0.04</v>
+      </c>
+      <c r="O35" s="17">
+        <v>0</v>
+      </c>
+      <c r="P35" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="16">
+        <v>2</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N36" s="17">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="O36" s="17">
+        <v>0</v>
+      </c>
+      <c r="P36" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="16">
+        <v>1</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="K37" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M37" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="N37" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="O37" s="17">
+        <v>0</v>
+      </c>
+      <c r="P37" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="16">
+        <v>1</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I38" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="N38" s="17">
+        <v>0.79</v>
+      </c>
+      <c r="O38" s="30">
+        <f>A38*N38</f>
+        <v>0.79</v>
+      </c>
+      <c r="P38" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="16">
+        <v>1</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="K39" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="N39" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="O39" s="17">
+        <v>1.02</v>
+      </c>
+      <c r="P39" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="16">
+        <v>1</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I40" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="J40" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="K40" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="N40" s="18">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="O40" s="17">
+        <v>0</v>
+      </c>
+      <c r="P40" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" location="common_component_prefixes" display="Reference Designator" xr:uid="{4147AC4C-D5EA-43D1-84FF-CD7C77D6B06E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F6 F7:F13 K39" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changers to the schematic, updated bom, and created priliminary layout for the PCB. Ready for 7B Prep!
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Dev\ECE445L\lab-7-and-10-project-nnat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11144611-5E22-49FB-A9F7-02A54F963FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D936EC-199E-4063-B93D-D1267AB17258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="3360" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
   </bookViews>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="346">
   <si>
     <t>Quantity</t>
   </si>
@@ -538,12 +538,6 @@
     <t>C5, C11</t>
   </si>
   <si>
-    <t>4.7u</t>
-  </si>
-  <si>
-    <t>C12, C13</t>
-  </si>
-  <si>
     <t>27n</t>
   </si>
   <si>
@@ -574,9 +568,6 @@
     <t>C19, C20, C31, C32</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4,  C14, C22, C23, C24, C25, C26, C33, C34, C35, C36, C37, C38</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -814,15 +805,6 @@
     <t>16V</t>
   </si>
   <si>
-    <t>GRM21BR71C475KE51L</t>
-  </si>
-  <si>
-    <t>81-GRM21BR71C475KE1L</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7UF 16V X7R 0805</t>
-  </si>
-  <si>
     <t>791-0603N100F500CT</t>
   </si>
   <si>
@@ -949,9 +931,6 @@
     <t>Thick FIlm</t>
   </si>
   <si>
-    <t>KOA Speer</t>
-  </si>
-  <si>
     <t>RK73B2ATTDD510J</t>
   </si>
   <si>
@@ -1042,9 +1021,6 @@
     <t>806-STX-3000</t>
   </si>
   <si>
-    <t>C21, C40</t>
-  </si>
-  <si>
     <t>R57, R81</t>
   </si>
   <si>
@@ -1091,18 +1067,6 @@
   </si>
   <si>
     <t>5POS</t>
-  </si>
-  <si>
-    <t>CONN PWR JACK 2.1X5.5MM SOLDER</t>
-  </si>
-  <si>
-    <t>Würth Elektronik</t>
-  </si>
-  <si>
-    <t>694106301002</t>
-  </si>
-  <si>
-    <t>710-694106301002</t>
   </si>
   <si>
     <r>
@@ -1172,6 +1136,207 @@
   </si>
   <si>
     <t>CAP TANT 2.2UF 10% 25V 1206</t>
+  </si>
+  <si>
+    <t>https://www.samsungsem.com/resources/file/global/support/product_catalog/MLCC.pdf</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/4819/TMK107B7105KA-T_SS.pdf</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM1885C1H103JA01-01.pdf</t>
+  </si>
+  <si>
+    <t>https://datasheets.kyocera-avx.com/F93.pdf</t>
+  </si>
+  <si>
+    <t>https://www.passivecomponent.com/wp-content/uploads/datasheet/WTC_MLCC_General_Purpose.pdf</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM1885C1H362JA01-01A.pdf</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM1885C1H122JA01-01.pdf</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/993/CL21B106KPQNNNE_Spec.pdf</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/SEI-RNCP.pdf</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/SEI-RNCF.pdf</t>
+  </si>
+  <si>
+    <t>https://www.yageogroup.com/content/datasheet/asset/file/PYU-RC_GROUP_51_ROHS_L</t>
+  </si>
+  <si>
+    <t>https://www.yageogroup.com/content/Resource%20Library/Datasheet/PYU-AF_51_ROHS_L.pdf</t>
+  </si>
+  <si>
+    <t>https://www.koaspeer.com/pdfs/RK73B.pdf</t>
+  </si>
+  <si>
+    <t>https://www.koaspeer.com/pdfs/RN73R.pdf</t>
+  </si>
+  <si>
+    <t>https://www.yageogroup.com/content/datasheet/asset/file/PYU-AC_51_ROHS_L</t>
+  </si>
+  <si>
+    <t>https://www.yageogroup.com/content/datasheet/asset/file/PYU-RC_51_ROHS_P</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/569/P120_Series_DS.pdf</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3, Q4, Q5, Q6, Q7, Q8, Q9, Q10, Q11, Q12, Q13, Q14, Q15, Q16, Q17, Q18</t>
+  </si>
+  <si>
+    <t>FET</t>
+  </si>
+  <si>
+    <t>MMBT2222ALT1G</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/3/101/1/MMBT2222LT1-D.PDF</t>
+  </si>
+  <si>
+    <t>npn</t>
+  </si>
+  <si>
+    <t>TRANS NPN 40V 0.6A SOT23-3</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tm4c123gh6pm.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1761592135417</t>
+  </si>
+  <si>
+    <t>https://documentation.espressif.com/esp32_datasheet_en.pdf</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/2289/FTDI_SmartBasic_Hookup_Guide.pdf</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/lm2937.pdf</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=10&amp;gotoUrl=https%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Ftlv5616</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=10&amp;gotoUrl=https%3A%2F%2Fwww.ti.com%2Flit%2Fgpn%2Flm4041c</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/opa350.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1761536704713&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Fopa350</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/datasheets/ST7735R_V0.2.pdf</t>
+  </si>
+  <si>
+    <t>https://users.ece.utexas.edu/%7Evalvano/Datasheets/1N914.pdf</t>
+  </si>
+  <si>
+    <t>https://users.ece.utexas.edu/%7Evalvano/Datasheets/LEDHLMP-D150.pdf</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-cs.com/media/wysiwyg/files/documentation/datasheet/boardwiretoboard/bwb_bergstik.pdf</t>
+  </si>
+  <si>
+    <t>https://www.kycon.com/Pub_Eng_Draw/STX-3000.pdf</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Resonators/ABM3.pdf</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>https://users.ece.utexas.edu/%7Evalvano/Datasheets/B3F-1059.pdf</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 24V</t>
+  </si>
+  <si>
+    <t>5ma</t>
+  </si>
+  <si>
+    <t>B3F-1000</t>
+  </si>
+  <si>
+    <t>Omron Electronics Inc-EMC Div</t>
+  </si>
+  <si>
+    <t>SW400-ND</t>
+  </si>
+  <si>
+    <t>863-MMBT2222ALT1G</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C12,  C14, C22, C23, C24, C25, C26, C33, C34, C35, C36, C37, C38</t>
+  </si>
+  <si>
+    <t>C13, C21, C40</t>
+  </si>
+  <si>
+    <t>R85, R86</t>
+  </si>
+  <si>
+    <t>5K1</t>
+  </si>
+  <si>
+    <t>2479774-1</t>
+  </si>
+  <si>
+    <t>571-2479774-1</t>
+  </si>
+  <si>
+    <t>USB-C CHARGE ONLY RECEPTACLE,6 P</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>TE Connectivity Linx</t>
+  </si>
+  <si>
+    <t>SW1, SW2, SW3, SW4, S5, SW6, SW7, SW8</t>
+  </si>
+  <si>
+    <t>SW9</t>
+  </si>
+  <si>
+    <t>SWITCH TOGGLE SPST 3A 125V</t>
+  </si>
+  <si>
+    <t>3A/125V</t>
+  </si>
+  <si>
+    <t>Adam Tech</t>
+  </si>
+  <si>
+    <t>SW-T3-1A-A-A3-S1</t>
+  </si>
+  <si>
+    <t>737-SW-T3-1A-A-A3-S1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/3/6015/1/sw-t3-1a-a-a3-s1-data-sheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=showdoc&amp;DocId=Data+Sheet%7Fdnd-fly-usb-type-c-charge-only-en-0324%7F2404%7Fpdf%7FEnglish%7FENG_DS_dnd-fly-usb-type-c-charge-only-en-0324_2404.pdf%7F2479774-1</t>
+  </si>
+  <si>
+    <t>RT0603FRD075K1L</t>
+  </si>
+  <si>
+    <t>603-RT0603FRD075K1L</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/3/508/1/PYu-RT_1-to-0.01_RoHS_L_15.pdf</t>
+  </si>
+  <si>
+    <t>RES SMD 5.1K OHM 1% 1/10W 0603</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1532,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1433,6 +1598,8 @@
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3320,10 +3487,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029DCE93-6AF6-4E19-8B76-EC8302CAC997}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3404,7 +3571,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="19" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="K3" s="19"/>
       <c r="L3" s="19"/>
@@ -3429,7 +3596,7 @@
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
       <c r="J4" s="24" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
@@ -3459,13 +3626,13 @@
         <v>83</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>6</v>
@@ -3494,10 +3661,10 @@
     </row>
     <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>105</v>
+        <v>324</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>82</v>
@@ -3506,7 +3673,7 @@
         <v>85</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F6" s="26" t="s">
         <v>84</v>
@@ -3515,32 +3682,35 @@
         <v>0.1</v>
       </c>
       <c r="H6" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M6" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="I6" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="N6" s="18">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="O6" s="18">
         <f>N6*A6</f>
-        <v>0.20799999999999999</v>
+        <v>0.221</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
@@ -3557,7 +3727,7 @@
         <v>86</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F7" s="26" t="s">
         <v>84</v>
@@ -3566,22 +3736,22 @@
         <v>0.1</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J7" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7" s="18" t="s">
         <v>169</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>172</v>
       </c>
       <c r="N7" s="18">
         <v>3.5999999999999997E-2</v>
@@ -3591,7 +3761,10 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
@@ -3599,7 +3772,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>82</v>
@@ -3608,7 +3781,7 @@
         <v>87</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>84</v>
@@ -3617,22 +3790,22 @@
         <v>0.05</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I8" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>181</v>
-      </c>
       <c r="K8" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N8" s="18">
         <v>5.0999999999999997E-2</v>
@@ -3642,7 +3815,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
@@ -3659,31 +3835,31 @@
         <v>88</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="G9" s="28">
         <v>0.1</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="N9" s="18">
         <v>2.08</v>
@@ -3693,7 +3869,10 @@
         <v>2.08</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
@@ -3710,7 +3889,7 @@
         <v>90</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>84</v>
@@ -3719,22 +3898,22 @@
         <v>0.01</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="N10" s="18">
         <v>2.5000000000000001E-2</v>
@@ -3744,15 +3923,18 @@
         <v>0.05</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>82</v>
@@ -3761,7 +3943,7 @@
         <v>93</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F11" s="26" t="s">
         <v>84</v>
@@ -3770,37 +3952,40 @@
         <v>0.1</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>185</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N11" s="18">
-        <v>5.1999999999999998E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O11" s="18">
-        <f>A11*N11</f>
-        <v>0.104</v>
+        <f t="shared" ref="O11:O26" si="1">A11*N11</f>
+        <v>0.1</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>101</v>
@@ -3809,61 +3994,64 @@
         <v>82</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F12" s="26" t="s">
         <v>84</v>
       </c>
       <c r="G12" s="28">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N12" s="18">
-        <v>2.5000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="O12" s="18">
-        <f t="shared" ref="O12:O26" si="1">A12*N12</f>
-        <v>0.1</v>
+        <f t="shared" si="1"/>
+        <v>0.08</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>84</v>
@@ -3872,151 +4060,160 @@
         <v>0.05</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I13" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>181</v>
-      </c>
       <c r="K13" s="18" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N13" s="18">
-        <v>0.04</v>
+        <v>2.7E-2</v>
       </c>
       <c r="O13" s="18">
         <f t="shared" si="1"/>
-        <v>0.08</v>
+        <v>0.108</v>
       </c>
       <c r="P13" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>104</v>
+        <v>325</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>84</v>
+      <c r="F14" s="18" t="s">
+        <v>122</v>
       </c>
       <c r="G14" s="28">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L14" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="N14" s="18">
-        <v>2.7E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="O14" s="18">
         <f t="shared" si="1"/>
-        <v>0.108</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="P14" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>261</v>
+        <v>120</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>125</v>
+      <c r="F15" s="26" t="s">
+        <v>84</v>
       </c>
       <c r="G15" s="28">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="H15" s="18" t="s">
         <v>201</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L15" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N15" s="18">
-        <v>2.3E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="O15" s="18">
         <f t="shared" si="1"/>
-        <v>4.5999999999999999E-2</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="P15" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F16" s="26" t="s">
         <v>84</v>
@@ -4025,46 +4222,49 @@
         <v>0.01</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="J16" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="K16" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="L16" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M16" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="L16" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M16" s="18" t="s">
-        <v>204</v>
-      </c>
       <c r="N16" s="18">
-        <v>8.9999999999999993E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="O16" s="18">
         <f t="shared" si="1"/>
-        <v>0.29699999999999999</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="P16" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>210</v>
@@ -4072,50 +4272,53 @@
       <c r="F17" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="28">
-        <v>0.01</v>
+      <c r="G17" s="29">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H17" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="K17" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="L17" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M17" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="J17" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="K17" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M17" s="18" t="s">
-        <v>209</v>
-      </c>
       <c r="N17" s="18">
-        <v>1.0999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="O17" s="18">
         <f t="shared" si="1"/>
-        <v>6.6000000000000003E-2</v>
+        <v>0.4</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>216</v>
@@ -4130,440 +4333,467 @@
         <v>215</v>
       </c>
       <c r="I18" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="K18" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="J18" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>213</v>
-      </c>
       <c r="L18" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M18" s="18" t="s">
         <v>212</v>
       </c>
       <c r="N18" s="18">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O18" s="18">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.06</v>
       </c>
       <c r="P18" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="C19" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>110</v>
-      </c>
       <c r="E19" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="29">
-        <v>5.0000000000000001E-3</v>
+      <c r="G19" s="28">
+        <v>0.01</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I19" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M19" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="J19" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>218</v>
-      </c>
       <c r="N19" s="18">
-        <v>1.4999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O19" s="18">
         <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="P19" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>2</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>262</v>
+        <v>113</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>112</v>
+        <v>106</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>153</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>84</v>
       </c>
       <c r="G20" s="28">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="K20" s="18" t="s">
         <v>224</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M20" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N20" s="18">
-        <v>1.2999999999999999E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="O20" s="18">
         <f t="shared" si="1"/>
-        <v>2.5999999999999999E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="P20" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>156</v>
+        <v>106</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>115</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="28">
-        <v>0.05</v>
+      <c r="G21" s="29">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="L21" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N21" s="18">
-        <v>2.5999999999999999E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="O21" s="18">
         <f t="shared" si="1"/>
-        <v>5.1999999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="P21" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>1</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="E22" s="18" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F22" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="29">
-        <v>5.0000000000000001E-3</v>
+      <c r="G22" s="28">
+        <v>0.01</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L22" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="N22" s="18">
-        <v>5.5E-2</v>
+        <v>0.06</v>
       </c>
       <c r="O22" s="18">
         <f t="shared" si="1"/>
-        <v>5.5E-2</v>
+        <v>0.06</v>
       </c>
       <c r="P22" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>1</v>
       </c>
       <c r="B23" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>120</v>
-      </c>
       <c r="E23" s="18" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F23" s="26" t="s">
         <v>84</v>
       </c>
       <c r="G23" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="N23" s="18">
         <v>0.01</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="J23" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="L23" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="M23" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="N23" s="18">
-        <v>0.06</v>
       </c>
       <c r="O23" s="18">
         <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="P23" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B24" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="D24" s="18" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="28">
-        <v>0.05</v>
+        <v>134</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>217</v>
+        <v>238</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>219</v>
+        <v>159</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M24" s="18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="N24" s="18">
-        <v>0.01</v>
+        <v>1.0169999999999999</v>
       </c>
       <c r="O24" s="18">
         <f t="shared" si="1"/>
+        <v>8.1359999999999992</v>
+      </c>
+      <c r="P24" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>2</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="28">
         <v>0.01</v>
       </c>
-      <c r="P24" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="18">
-        <v>8</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>128</v>
-      </c>
       <c r="H25" s="18" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>161</v>
+        <v>240</v>
       </c>
       <c r="L25" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N25" s="18">
-        <v>1.0169999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="O25" s="18">
         <f t="shared" si="1"/>
-        <v>8.1359999999999992</v>
+        <v>0.02</v>
       </c>
       <c r="P25" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>2</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>145</v>
+        <v>326</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>155</v>
+        <v>327</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="F26" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="F26" s="26" t="s">
         <v>84</v>
       </c>
       <c r="G26" s="28">
         <v>0.01</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>246</v>
+        <v>342</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>247</v>
+        <v>343</v>
       </c>
       <c r="N26" s="18">
-        <v>0.01</v>
+        <v>3.1E-2</v>
       </c>
       <c r="O26" s="18">
         <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>6.2E-2</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="16">
         <v>1</v>
       </c>
@@ -4574,20 +4804,20 @@
         <v>13</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>38</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>14</v>
@@ -4610,8 +4840,11 @@
       <c r="P27" s="18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q27" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="16">
         <v>1</v>
       </c>
@@ -4622,22 +4855,22 @@
         <v>13</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J28" s="16" t="s">
         <v>50</v>
@@ -4658,10 +4891,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="18" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="16">
         <v>1</v>
       </c>
@@ -4672,20 +4908,20 @@
         <v>10</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>54</v>
       </c>
       <c r="F29" s="18"/>
       <c r="G29" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J29" s="16" t="s">
         <v>58</v>
@@ -4706,10 +4942,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="16">
         <v>1</v>
       </c>
@@ -4720,34 +4959,34 @@
         <v>10</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E30" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="I30" s="16" t="s">
         <v>127</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>130</v>
       </c>
       <c r="J30" s="16" t="s">
         <v>14</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L30" s="16" t="s">
         <v>29</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N30" s="17">
         <v>1.45</v>
@@ -4758,34 +4997,37 @@
       <c r="P30" s="18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q30" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
         <v>2</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>14</v>
@@ -4808,8 +5050,11 @@
       <c r="P31" s="18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q31" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="16">
         <v>1</v>
       </c>
@@ -4820,22 +5065,22 @@
         <v>10</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>14</v>
@@ -4858,10 +5103,13 @@
       <c r="P32" s="18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>80</v>
@@ -4870,22 +5118,22 @@
         <v>10</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>14</v>
@@ -4906,48 +5154,51 @@
         <v>0</v>
       </c>
       <c r="P33" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="16">
         <v>1</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="L34" s="16" t="s">
         <v>9</v>
       </c>
       <c r="M34" s="18" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="N34" s="17">
         <v>34.950000000000003</v>
@@ -4958,46 +5209,49 @@
       <c r="P34" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="Q34" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="16">
         <v>2</v>
       </c>
       <c r="B35" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="F35" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="G35" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H35" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="I35" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="J35" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="K35" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="G35" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H35" s="16" t="s">
+      <c r="L35" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="I35" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="K35" s="18" t="s">
+      <c r="M35" s="18" t="s">
         <v>140</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="M35" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="N35" s="17">
         <v>0.04</v>
@@ -5006,48 +5260,51 @@
         <v>0</v>
       </c>
       <c r="P35" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="16">
         <v>2</v>
       </c>
       <c r="B36" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="F36" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="G36" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J36" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I36" s="18" t="s">
+      <c r="K36" s="18" t="s">
         <v>150</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>153</v>
       </c>
       <c r="L36" s="16" t="s">
         <v>9</v>
       </c>
       <c r="M36" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="N36" s="17">
         <v>0.40200000000000002</v>
@@ -5056,48 +5313,51 @@
         <v>0</v>
       </c>
       <c r="P36" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="16">
         <v>1</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="L37" s="16" t="s">
         <v>52</v>
       </c>
       <c r="M37" s="18" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="N37" s="17">
         <v>0.1</v>
@@ -5106,48 +5366,51 @@
         <v>0</v>
       </c>
       <c r="P37" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="16">
         <v>1</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="K38" s="18" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M38" s="18" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="N38" s="17">
         <v>0.79</v>
@@ -5157,96 +5420,105 @@
         <v>0.79</v>
       </c>
       <c r="P38" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="16">
         <v>1</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="D39" s="18"/>
+        <v>156</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>125</v>
+      </c>
       <c r="E39" s="18" t="s">
-        <v>278</v>
+        <v>330</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>128</v>
+        <v>331</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>279</v>
+        <v>332</v>
       </c>
       <c r="K39" s="26" t="s">
-        <v>280</v>
+        <v>328</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M39" s="18" t="s">
-        <v>281</v>
+        <v>329</v>
       </c>
       <c r="N39" s="17">
-        <v>1.02</v>
+        <v>0.61</v>
       </c>
       <c r="O39" s="17">
-        <v>1.02</v>
+        <f>A39*N39</f>
+        <v>0.61</v>
       </c>
       <c r="P39" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="16">
         <v>1</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="K40" s="18" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="L40" s="16" t="s">
         <v>9</v>
       </c>
       <c r="M40" s="18" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="N40" s="18">
         <v>0.83099999999999996</v>
@@ -5255,26 +5527,172 @@
         <v>0</v>
       </c>
       <c r="P40" s="18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
+        <v>243</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="16">
+        <v>18</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="M41" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="N41" s="17">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="O41" s="31">
+        <f>A41*N41</f>
+        <v>1.5839999999999999</v>
+      </c>
+      <c r="P41" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="16">
+        <v>8</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" t="s">
+        <v>318</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J42" t="s">
+        <v>321</v>
+      </c>
+      <c r="K42" t="s">
+        <v>320</v>
+      </c>
+      <c r="L42" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" t="s">
+        <v>322</v>
+      </c>
+      <c r="N42" s="17">
+        <v>0</v>
+      </c>
+      <c r="O42" s="17">
+        <v>0</v>
+      </c>
+      <c r="P42" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="16">
+        <v>1</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J43" t="s">
+        <v>337</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="L43" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="M43" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="N43" s="17">
+        <v>0.98</v>
+      </c>
+      <c r="O43" s="32">
+        <f>A43*N43</f>
+        <v>0.98</v>
+      </c>
+      <c r="P43" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>340</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5282,7 +5700,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F6 F7:F13 K39" numberStoredAsText="1"/>
+    <ignoredError sqref="F6 F7:F10 F11:F12" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Rough draft layout - need to remove tm4c chip
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Dev\ECE445L\lab-7-and-10-project-nnat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D936EC-199E-4063-B93D-D1267AB17258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E06A43-C14E-40EE-AF86-61CA63B44AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="3360" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
   </bookViews>
@@ -3490,7 +3490,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added current consumption to schematic
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Dev\ECE445L\lab-7-and-10-project-nnat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E06A43-C14E-40EE-AF86-61CA63B44AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BB960D-3F3E-4F32-B8DD-CFFD2D76AD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="3360" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -2015,21 +2015,21 @@
       <selection activeCell="P23" sqref="A1:P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="65.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="65.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.453125" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="24.54296875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -2063,7 +2063,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2075,7 +2075,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>7</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -2402,12 +2402,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>16</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>8</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D22" s="3" t="s">
         <v>71</v>
       </c>
@@ -2491,275 +2491,275 @@
       <c r="F22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:8" x14ac:dyDescent="0.35">
       <c r="F80" s="1"/>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="H84" s="11"/>
@@ -2789,15 +2789,15 @@
       <selection activeCell="A6" sqref="A6:K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="70.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2867,7 +2867,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -2891,7 +2891,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +2933,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -3013,7 +3013,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -3081,7 +3081,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>7</v>
       </c>
@@ -3204,7 +3204,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>16</v>
       </c>
@@ -3300,7 +3300,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>8</v>
       </c>
@@ -3334,7 +3334,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -3364,7 +3364,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3382,7 +3382,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3400,7 +3400,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -3418,7 +3418,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3436,7 +3436,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3456,7 +3456,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3487,28 +3487,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029DCE93-6AF6-4E19-8B76-EC8302CAC997}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="51" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.54296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
@@ -3535,7 +3535,7 @@
       <c r="P1" s="18"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>48</v>
       </c>
@@ -3560,7 +3560,7 @@
       <c r="P2" s="18"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -3581,7 +3581,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>24</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18">
         <v>17</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>2</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>4</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>2</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>4</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>2</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>4</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="18">
         <v>3</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="18">
         <v>33</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>6</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>20</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>4</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>2</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>2</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>1</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>1</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>1</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>8</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="18">
         <v>2</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>2</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="16">
         <v>1</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="16">
         <v>1</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>1</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="16">
         <v>1</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
         <v>2</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="16">
         <v>1</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="16">
         <v>8</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <v>1</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="16">
         <v>2</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="16">
         <v>2</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="16">
         <v>1</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="16">
         <v>1</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="16">
         <v>1</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="16">
         <v>1</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="16">
         <v>18</v>
       </c>
@@ -5587,7 +5587,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="16">
         <v>8</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="16">
         <v>1</v>
       </c>
@@ -5692,6 +5692,12 @@
       </c>
       <c r="Q43" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <f>SUM(O6:O43)</f>
+        <v>16.191999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated bom for lab 7B
</commit_message>
<xml_diff>
--- a/Lab7BOM.xlsx
+++ b/Lab7BOM.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Dev\ECE445L\lab-7-and-10-project-nnat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1144435A-515C-4686-89FE-6483DAF64C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F5A3C8-8909-4B56-9816-AD7AC155568C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
+    <workbookView xWindow="-38520" yWindow="3360" windowWidth="38640" windowHeight="21120" xr2:uid="{2A746B91-5B93-4559-A98B-A0C4C3CDA5C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM_NEW" sheetId="5" r:id="rId1"/>
-    <sheet name="BOM_OLD" sheetId="4" r:id="rId2"/>
+    <sheet name="BOM_NEW_2" sheetId="6" r:id="rId1"/>
+    <sheet name="BOM_NEW" sheetId="5" r:id="rId2"/>
+    <sheet name="BOM_OLD" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,6 +35,65 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ECE_IT</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{0C06522C-C06C-4B62-B92E-8C488D4FBBCA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ECE_IT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+How many are on your board. If 0, it should probably not clutter your bom up…
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{FFB429E3-CDB9-4034-B3E1-3C56792C2522}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ECE_IT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is something like C1, R2 , U1, etc. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ECE_IT</author>
@@ -92,7 +152,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>ECE_IT</author>
@@ -152,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="449">
   <si>
     <t>Quantity</t>
   </si>
@@ -1316,6 +1376,231 @@
   </si>
   <si>
     <t>RES 3.3K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>C2, C14, C26</t>
+  </si>
+  <si>
+    <t>C4, C6, C16, C18</t>
+  </si>
+  <si>
+    <t>C5, C7, C17, C19</t>
+  </si>
+  <si>
+    <t>C8, C20</t>
+  </si>
+  <si>
+    <t>C9, C21</t>
+  </si>
+  <si>
+    <t>C1, C3, C9, C10, C11, C12, C13, C15, C21, C22, C23, C24, C25, C27,C28, C29, C30, C31, C32, C33, C34</t>
+  </si>
+  <si>
+    <t>D1, D2, D5</t>
+  </si>
+  <si>
+    <t>MMBF-170</t>
+  </si>
+  <si>
+    <t>R5, R9, R10, R12, R20, R21, R31, R33, R35, R36, R42, R43, R46, R53, R54, R62, R64, R65, R67</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R27, R29</t>
+  </si>
+  <si>
+    <t>R11, R13, R22, R23, R24, R32, R44, R45, R56, R57, R63, R103, R104, R105, R109, R110, R111</t>
+  </si>
+  <si>
+    <t>184k</t>
+  </si>
+  <si>
+    <t>R14, R25, R47, R58</t>
+  </si>
+  <si>
+    <t>R15, R26, R48, R59</t>
+  </si>
+  <si>
+    <t>68.8k</t>
+  </si>
+  <si>
+    <t>R16, R17, R28, R37, R49, R50, R60, R68</t>
+  </si>
+  <si>
+    <t>R18, R19, R30, R51, R52, R61</t>
+  </si>
+  <si>
+    <t>R34, R66</t>
+  </si>
+  <si>
+    <t>R38, R69</t>
+  </si>
+  <si>
+    <t>R39, R40, R70, R71</t>
+  </si>
+  <si>
+    <t>R51, R72</t>
+  </si>
+  <si>
+    <t>50k</t>
+  </si>
+  <si>
+    <t>R73, R75, R77, R79, R81, R84, R88</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>R74, R76, R78, R80, R85, R89, R101, R107</t>
+  </si>
+  <si>
+    <t>R83, R86, R87, R90, R91, R92, R93, R94</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>R96, R97</t>
+  </si>
+  <si>
+    <t>R95, R98, R99</t>
+  </si>
+  <si>
+    <t>U5, U6, U7, U8, U10, U11, U12, U13</t>
+  </si>
+  <si>
+    <t>U9, U14</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>512-MMBF170</t>
+  </si>
+  <si>
+    <t>N-Channel 60 V 500mA (Ta) 300mW (Ta) Surface Mount SOT-23-3</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>n-type</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/mmbf170-d.pdf</t>
+  </si>
+  <si>
+    <t>RT0603DRE07184KL</t>
+  </si>
+  <si>
+    <t>603-RT0603DRE07184KL</t>
+  </si>
+  <si>
+    <t>RES 184K OHM 0.5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>ERA-3AEB6812V</t>
+  </si>
+  <si>
+    <t>667-ERA-3AEB6812V</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>RES SMD 68.1KOHM 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDM0000/AOA0000C307.pdf</t>
+  </si>
+  <si>
+    <t>https://www.yageogroup.com/browse/products?search=pyu-rt_1-to-0.01_rohs_l.pdf</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE0730KL</t>
+  </si>
+  <si>
+    <t>RT0603FRE0730KL</t>
+  </si>
+  <si>
+    <t>RES SMD 30K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>RT0603DRD0749K9L</t>
+  </si>
+  <si>
+    <t>603-RT0603DRD0749K9L</t>
+  </si>
+  <si>
+    <t>RES SMD 49.9KOHM 0.5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R100, R106</t>
+  </si>
+  <si>
+    <t>R102, R108</t>
+  </si>
+  <si>
+    <t>75R</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>176R</t>
+  </si>
+  <si>
+    <t>660-RN73H1JTD1760D25</t>
+  </si>
+  <si>
+    <t>RN73H1JTTD1760D25</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/catalog/specsheets/KOA_Speer_RN73H_8_21_24.pdf</t>
+  </si>
+  <si>
+    <t>RES 176 OHM 0.5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>MCT0603PD1000DP500</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/28916/mcxhp.pdf</t>
+  </si>
+  <si>
+    <t>594-MCT0603PD1000DP5</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 0.5% 1/4W 0603</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE101K5L</t>
+  </si>
+  <si>
+    <t>RT0603FRE101K5L</t>
+  </si>
+  <si>
+    <t>RES 1.5K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RP73PF1J75RBTDF</t>
+  </si>
+  <si>
+    <t>TE Connectivity / Holsworthy</t>
+  </si>
+  <si>
+    <t>279-RP73PF1J75RBTDF</t>
+  </si>
+  <si>
+    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=showdoc&amp;DocId=Data+Sheet%7F1773272%7FL%7Fpdf%7FEnglish%7FENG_DS_1773272_L.pdf%7F</t>
+  </si>
+  <si>
+    <t>RES SMD 75 OHM 0.1% 1/6W 0603</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1749,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1507,6 +1792,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1915,10 +2201,2635 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FB3CFA1-E3EF-4F3F-9852-4595399E539B}">
+  <dimension ref="A1:S66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S58" sqref="S58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10">
+        <v>45968</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="9"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="N6" s="8">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O6" s="8">
+        <f>A6*N6</f>
+        <v>0.247</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="N7" s="8">
+        <v>2.3E-2</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" ref="O7:O47" si="0">A7*N7</f>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="23">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="N8" s="8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.108</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="N9" s="8">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.128</v>
+      </c>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="N10" s="8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="23">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0.61</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="23">
+        <v>1</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="23">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="O16" s="8">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="23">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0.158</v>
+      </c>
+      <c r="O17" s="8">
+        <f t="shared" si="0"/>
+        <v>2.528</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="23">
+        <v>2</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="N18" s="8">
+        <v>3.1E-2</v>
+      </c>
+      <c r="O18" s="8">
+        <f t="shared" si="0"/>
+        <v>6.2E-2</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="23">
+        <v>1</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="N19" s="8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="O19" s="8">
+        <f t="shared" si="0"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="23">
+        <v>1</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="N20" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="O20" s="8">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="23">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="N21" s="8">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O21" s="8">
+        <f t="shared" si="0"/>
+        <v>0.17099999999999999</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q21" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="23">
+        <v>5</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="N22" s="8">
+        <v>2.7E-2</v>
+      </c>
+      <c r="O22" s="8">
+        <f t="shared" si="0"/>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q22" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="23">
+        <v>18</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="O23" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q23" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="23">
+        <v>4</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="N24" s="8">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O24" s="8">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="23">
+        <v>4</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="N25" s="8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="O25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.216</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q25" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="23">
+        <v>8</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="N26" s="8">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="O26" s="8">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="P26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q26" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="23">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="N27" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O27" s="8">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q27" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="23">
+        <v>2</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="N28" s="8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="O28" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="23">
+        <v>2</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="N29" s="8">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O29" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4E-2</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="23">
+        <v>4</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="N30" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O30" s="8">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q30" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="23">
+        <v>2</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="N31" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="O31" s="8">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q31" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="23">
+        <v>7</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="N32" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="O32" s="8">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+    </row>
+    <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="23">
+        <v>8</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="N33" s="8">
+        <v>9.4E-2</v>
+      </c>
+      <c r="O33" s="8">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="P33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q33" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="23">
+        <v>8</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M34" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="N34" s="8">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="O34" s="8">
+        <f t="shared" si="0"/>
+        <v>8.1359999999999992</v>
+      </c>
+      <c r="P34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q34" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+    </row>
+    <row r="35" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="23">
+        <v>3</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="N35" s="8">
+        <v>1.6E-2</v>
+      </c>
+      <c r="O35" s="8">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q35" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="23">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="N36" s="8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O36" s="8">
+        <f t="shared" si="0"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q36" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+    </row>
+    <row r="37" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="23">
+        <v>2</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>432</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="N37" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="O37" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q37" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+    </row>
+    <row r="38" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="23">
+        <v>2</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>430</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="F38" s="16">
+        <v>603</v>
+      </c>
+      <c r="G38" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="N38" s="8">
+        <v>0.215</v>
+      </c>
+      <c r="O38" s="8">
+        <f t="shared" si="0"/>
+        <v>0.43</v>
+      </c>
+      <c r="P38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q38" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+    </row>
+    <row r="39" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="23">
+        <v>1</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="N39" s="7">
+        <v>0.98</v>
+      </c>
+      <c r="O39" s="8">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="P39" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q39" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="23">
+        <v>7</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="N40" s="7">
+        <v>0</v>
+      </c>
+      <c r="O40" s="8">
+        <v>0</v>
+      </c>
+      <c r="P40" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q40" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A41" s="23">
+        <v>1</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N41" s="7">
+        <v>1.45</v>
+      </c>
+      <c r="O41" s="8">
+        <v>0</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q41" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="23">
+        <v>1</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N42" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="O42" s="8">
+        <v>0</v>
+      </c>
+      <c r="P42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q42" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+    </row>
+    <row r="43" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A43" s="23">
+        <v>1</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N43" s="7">
+        <v>1.68</v>
+      </c>
+      <c r="O43" s="8">
+        <v>0</v>
+      </c>
+      <c r="P43" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q43" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A44" s="23">
+        <v>1</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K44" s="6">
+        <v>12935</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O44" s="8">
+        <v>0</v>
+      </c>
+      <c r="P44" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q44" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+    </row>
+    <row r="45" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="23">
+        <v>8</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N45" s="2">
+        <v>3.9089999999999998</v>
+      </c>
+      <c r="O45" s="8">
+        <v>0</v>
+      </c>
+      <c r="P45" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q45" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A46" s="23">
+        <v>2</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N46" s="7">
+        <v>11.06</v>
+      </c>
+      <c r="O46" s="8">
+        <v>0</v>
+      </c>
+      <c r="P46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q46" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+    </row>
+    <row r="47" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="23">
+        <v>1</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="N47" s="7">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="O47" s="8">
+        <v>0</v>
+      </c>
+      <c r="P47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q47" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+    </row>
+    <row r="48" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A48" s="23"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="7">
+        <f>SUM(O6:O47)</f>
+        <v>17.009</v>
+      </c>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+    </row>
+    <row r="49" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+    </row>
+    <row r="54" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="23"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+    </row>
+    <row r="63" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+    </row>
+    <row r="65" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A65" s="23"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="23"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="8"/>
+      <c r="N66" s="8"/>
+      <c r="O66" s="8"/>
+      <c r="P66" s="8"/>
+      <c r="Q66" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" location="common_component_prefixes" display="Reference Designator" xr:uid="{07EB1CDF-FAEA-4EC4-A795-07D494C842C8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3D64F8-5E1F-4E3A-9888-F591BAAE8F3C}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
@@ -4365,7 +7276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029DCE93-6AF6-4E19-8B76-EC8302CAC997}">
   <dimension ref="A1:Q44"/>
   <sheetViews>

</xml_diff>